<commit_message>
Test cases added for Mercedes, test data and test steps also added.
</commit_message>
<xml_diff>
--- a/com.mbusa/src/test/resources/test_data.xlsx
+++ b/com.mbusa/src/test/resources/test_data.xlsx
@@ -5,17 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yahya\IdeaProjects\SeleniumBootcamp\com.marketwatch\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yahya\IdeaProjects\SeleniumBootcamp\com.mbusa\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F3AAF62-DE91-4581-80EF-C82E2506AC74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE82D24E-6717-4B0E-B942-D0AC29C16858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" activeTab="2" xr2:uid="{5DC96F64-0600-4540-8EF4-E6AE23C27A48}"/>
+    <workbookView xWindow="4240" yWindow="0" windowWidth="17140" windowHeight="14320" xr2:uid="{5DC96F64-0600-4540-8EF4-E6AE23C27A48}"/>
   </bookViews>
   <sheets>
-    <sheet name="USMarket" sheetId="1" r:id="rId1"/>
-    <sheet name="EuropeMarket" sheetId="2" r:id="rId2"/>
-    <sheet name="AsiaMarket" sheetId="3" r:id="rId3"/>
+    <sheet name="AMG" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,63 +35,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Assertions</t>
   </si>
   <si>
-    <t>Dow Jones Industrial Average</t>
+    <t>MERCEDES-AMG ENGINES</t>
   </si>
   <si>
-    <t>S&amp;P 500 Index</t>
-  </si>
-  <si>
-    <t>NASDAQ Composite Index</t>
-  </si>
-  <si>
-    <t>Global Dow Realtime USD</t>
-  </si>
-  <si>
-    <t>Gold Continuous Contract</t>
-  </si>
-  <si>
-    <t>Crude Oil WTI (NYM $/bbl) Front Month</t>
-  </si>
-  <si>
-    <t>FTSE 100 Index</t>
-  </si>
-  <si>
-    <t>DAX</t>
-  </si>
-  <si>
-    <t>CAC 40 Index</t>
-  </si>
-  <si>
-    <t>FTSE MIB Index</t>
-  </si>
-  <si>
-    <t>IBEX 35 Index</t>
-  </si>
-  <si>
-    <t>STOXX Europe 600 Index</t>
-  </si>
-  <si>
-    <t>The Asia Dow Index USD</t>
-  </si>
-  <si>
-    <t>NIKKEI 225 Index</t>
-  </si>
-  <si>
-    <t>Hang Seng Index</t>
-  </si>
-  <si>
-    <t>Shanghai Composite Index</t>
-  </si>
-  <si>
-    <t>S&amp;P BSE Sensex Index</t>
-  </si>
-  <si>
-    <t>FTSE Straits Times Index</t>
+    <t>PERFORMANCE 6/6</t>
   </si>
 </sst>
 </file>
@@ -455,11 +405,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06C7C825-8D82-4132-9F2A-6781F4BC04E3}">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
@@ -478,134 +430,18 @@
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="A4" s="1"/>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A5" s="1"/>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="A6" s="1"/>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="A7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{641687E4-DD92-495D-B79E-84D3197FD0E8}">
-  <dimension ref="A1:A7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="21.36328125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8B39C1C-9BB3-40D5-A3B2-012E20FAD986}">
-  <dimension ref="A1:A7"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="23.08984375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
added assertion to test case to rotate animation for mercedes.
</commit_message>
<xml_diff>
--- a/com.mbusa/src/test/resources/test_data.xlsx
+++ b/com.mbusa/src/test/resources/test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yahya\IdeaProjects\SeleniumBootcamp\com.mbusa\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE82D24E-6717-4B0E-B942-D0AC29C16858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B2FC48D-9647-4437-AFB7-94E06B4283CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4240" yWindow="0" windowWidth="17140" windowHeight="14320" xr2:uid="{5DC96F64-0600-4540-8EF4-E6AE23C27A48}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Assertions</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t>PERFORMANCE 6/6</t>
+  </si>
+  <si>
+    <t>Mercedes-AMG Design: explore the possibilities.</t>
   </si>
 </sst>
 </file>
@@ -406,12 +409,12 @@
   <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
@@ -430,7 +433,9 @@
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>

</xml_diff>

<commit_message>
added test cases to mercedes.
</commit_message>
<xml_diff>
--- a/com.mbusa/src/test/resources/test_data.xlsx
+++ b/com.mbusa/src/test/resources/test_data.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yahya\IdeaProjects\SeleniumBootcamp\com.mbusa\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B2FC48D-9647-4437-AFB7-94E06B4283CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D972EA1-A1FD-4CD2-8D28-AD04418E7AD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4240" yWindow="0" windowWidth="17140" windowHeight="14320" xr2:uid="{5DC96F64-0600-4540-8EF4-E6AE23C27A48}"/>
+    <workbookView xWindow="4240" yWindow="0" windowWidth="17140" windowHeight="14320" activeTab="2" xr2:uid="{5DC96F64-0600-4540-8EF4-E6AE23C27A48}"/>
   </bookViews>
   <sheets>
     <sheet name="AMG" sheetId="1" r:id="rId1"/>
+    <sheet name="Shopping" sheetId="2" r:id="rId2"/>
+    <sheet name="Inventory" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Assertions</t>
   </si>
@@ -43,10 +45,34 @@
     <t>MERCEDES-AMG ENGINES</t>
   </si>
   <si>
-    <t>PERFORMANCE 6/6</t>
-  </si>
-  <si>
     <t>Mercedes-AMG Design: explore the possibilities.</t>
+  </si>
+  <si>
+    <t>Compare Vehicles</t>
+  </si>
+  <si>
+    <t>New Vehicle Inventory</t>
+  </si>
+  <si>
+    <t>Certified Pre-Owned Inventory</t>
+  </si>
+  <si>
+    <t>Discover the Lineup</t>
+  </si>
+  <si>
+    <t>PERFORMANCE 2/6</t>
+  </si>
+  <si>
+    <t>What Makes a CPO Vehicle Certified?</t>
+  </si>
+  <si>
+    <t>The Certified Pre-Owned Limited Warranty</t>
+  </si>
+  <si>
+    <t>Build Your Deal</t>
+  </si>
+  <si>
+    <t>Special Offers &amp; More</t>
   </si>
 </sst>
 </file>
@@ -408,7 +434,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06C7C825-8D82-4132-9F2A-6781F4BC04E3}">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -429,12 +455,12 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
@@ -445,6 +471,92 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74237377-1558-404F-A338-05B53C57920A}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E4E158C-B943-4ECF-9368-D35FEB09C1BB}">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="31.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>